<commit_message>
red cross app designer changes
</commit_message>
<xml_diff>
--- a/app/config/tables/deployment/forms/deployment/deployment.xlsx
+++ b/app/config/tables/deployment/forms/deployment/deployment.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4280" yWindow="5660" windowWidth="31300" windowHeight="16100" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="-80" yWindow="3680" windowWidth="50300" windowHeight="19840" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="model" sheetId="2" r:id="rId1"/>
     <sheet name="settings" sheetId="3" r:id="rId2"/>
     <sheet name="survey" sheetId="1" r:id="rId3"/>
-    <sheet name="choices" sheetId="4" r:id="rId4"/>
-    <sheet name="queries" sheetId="6" r:id="rId5"/>
+    <sheet name="queries" sheetId="6" r:id="rId4"/>
+    <sheet name="choices" sheetId="4" r:id="rId5"/>
     <sheet name="prompt_types" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="109">
   <si>
     <t>type</t>
   </si>
@@ -137,15 +137,6 @@
     <t>distribution</t>
   </si>
   <si>
-    <t>beneficiary_code = ?</t>
-  </si>
-  <si>
-    <t>[data('beneficiary_code')]</t>
-  </si>
-  <si>
-    <t>'beneficiary_code='+opendatakit.encodeURIDataElement('beneficiary_code')</t>
-  </si>
-  <si>
     <t>deployment_info</t>
   </si>
   <si>
@@ -185,9 +176,6 @@
     <t>note</t>
   </si>
   <si>
-    <t>Please continue to fill out final distribution report</t>
-  </si>
-  <si>
     <t>end screen</t>
   </si>
   <si>
@@ -207,13 +195,169 @@
   </si>
   <si>
     <t>'beneficiary_code='+opendatakit.encodeURIDataElement('beneficiary_code')+ '&amp;_id='+opendatakit.encodeURIDataElement('distribution_row_id')</t>
+  </si>
+  <si>
+    <t>if</t>
+  </si>
+  <si>
+    <t>assign</t>
+  </si>
+  <si>
+    <t>calculation</t>
+  </si>
+  <si>
+    <t>now()</t>
+  </si>
+  <si>
+    <t>What is the name of the distributor?</t>
+  </si>
+  <si>
+    <t>pre-summary</t>
+  </si>
+  <si>
+    <t>Since the authorized item pack was successfully distributed, we will complete now complete a brief report.</t>
+  </si>
+  <si>
+    <t>What is the name of the distribution site?</t>
+  </si>
+  <si>
+    <t>thanks</t>
+  </si>
+  <si>
+    <t>Thank you for completing the post-distribution survey. Continue to the next screen to finalize.</t>
+  </si>
+  <si>
+    <t>else</t>
+  </si>
+  <si>
+    <t>end if</t>
+  </si>
+  <si>
+    <t>data('is_distributed') == 'true'</t>
+  </si>
+  <si>
+    <t>beneficiary_code = ? and is_distributed = ?</t>
+  </si>
+  <si>
+    <t>[data('beneficiary_code'), 'false']</t>
+  </si>
+  <si>
+    <t>'beneficiary_code='+opendatakit.encodeURIDataElement('beneficiary_code')+ '&amp;is_distributed='+opendatakit.encodeURIValue('false')</t>
+  </si>
+  <si>
+    <t>Please continue to distribute item pack and fill out final distribution report</t>
+  </si>
+  <si>
+    <t>min_range_query</t>
+  </si>
+  <si>
+    <t>beneficiary_code = ? and _id = ?</t>
+  </si>
+  <si>
+    <t>min_range</t>
+  </si>
+  <si>
+    <t>max_range_query</t>
+  </si>
+  <si>
+    <t>max_range</t>
+  </si>
+  <si>
+    <t>model.isSessionVariable</t>
+  </si>
+  <si>
+    <t>pre-deployment</t>
+  </si>
+  <si>
+    <t>We will now distribute the appropriate item pack</t>
+  </si>
+  <si>
+    <t>item_pack_barcode</t>
+  </si>
+  <si>
+    <t>(data('scanned_item_pack_barcode') &gt; data('maxRange')) || (data('scanned_item_pack_barcode') &lt; data('minRange'))</t>
+  </si>
+  <si>
+    <t>yes_no</t>
+  </si>
+  <si>
+    <t>try_again</t>
+  </si>
+  <si>
+    <t>Unauthorized Item Pack! Do not distribute this  item pack. Would you like to scan a different item pack?</t>
+  </si>
+  <si>
+    <t>selected(data('try_again'),'yes')</t>
+  </si>
+  <si>
+    <t>goto item_scan</t>
+  </si>
+  <si>
+    <t>This item pack is authorized. Please distribute this item pack.</t>
+  </si>
+  <si>
+    <t>branch_label</t>
+  </si>
+  <si>
+    <t>item_scan</t>
+  </si>
+  <si>
+    <t>Would you like to scan a different item pack instead?</t>
+  </si>
+  <si>
+    <t>true_false</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>no_report_option</t>
+  </si>
+  <si>
+    <t>Since no item pack was successfully distributed, we will not fill out a post-distribution report.</t>
+  </si>
+  <si>
+    <t>Please click the pencil icon to record distribution</t>
+  </si>
+  <si>
+    <t>Please continue to the next screen if you have clicked the pencil icon to record distribution</t>
+  </si>
+  <si>
+    <t>set_is_distributed</t>
+  </si>
+  <si>
+    <t>is_distributed_value_query</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>Scan an item pack barcode within the range of {{data.min_range}} to {{data.max_range}}</t>
+  </si>
+  <si>
+    <t>No authorized item pack was selected</t>
+  </si>
+  <si>
+    <t>data('distribution_id') != ''</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -264,8 +408,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -320,6 +470,24 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6600"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -358,7 +526,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -382,8 +550,22 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -408,8 +590,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="37">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -421,6 +614,13 @@
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -432,6 +632,13 @@
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -761,10 +968,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="26" defaultRowHeight="23" x14ac:dyDescent="0"/>
@@ -819,7 +1026,15 @@
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>56</v>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -912,29 +1127,30 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="23" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="24.33203125" customWidth="1"/>
+    <col min="1" max="1" width="17" style="7" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" style="7" customWidth="1"/>
     <col min="3" max="3" width="35.5" style="4" customWidth="1"/>
     <col min="4" max="4" width="38.1640625" style="4" customWidth="1"/>
     <col min="5" max="5" width="56.1640625" style="5" customWidth="1"/>
     <col min="6" max="6" width="64.33203125" style="13" customWidth="1"/>
     <col min="7" max="7" width="42.1640625" style="16" customWidth="1"/>
+    <col min="8" max="8" width="42.1640625" style="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:10">
       <c r="A1" s="9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -951,8 +1167,17 @@
       <c r="G1" s="14" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="I1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="C2" s="4" t="s">
         <v>4</v>
       </c>
@@ -963,8 +1188,9 @@
         <v>25</v>
       </c>
       <c r="G2" s="15"/>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="H2" s="24"/>
+    </row>
+    <row r="3" spans="1:10">
       <c r="C3" s="4" t="s">
         <v>2</v>
       </c>
@@ -975,83 +1201,400 @@
         <v>26</v>
       </c>
       <c r="G3" s="15"/>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="H3" s="24"/>
+    </row>
+    <row r="4" spans="1:10">
       <c r="C4" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G4" s="15"/>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="H4" s="24"/>
+    </row>
+    <row r="5" spans="1:10">
       <c r="C5" s="4" t="s">
         <v>35</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G5" s="15"/>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
-        <v>51</v>
+      <c r="H5" s="24"/>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="7" t="s">
+        <v>48</v>
       </c>
       <c r="F6" s="12"/>
       <c r="G6" s="15"/>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="H6" s="24"/>
+    </row>
+    <row r="7" spans="1:10">
       <c r="C7" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="G7" s="15"/>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="H7" s="24"/>
+    </row>
+    <row r="8" spans="1:10">
       <c r="C8" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:10">
       <c r="C9" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="19" spans="5:6">
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
+        <v>76</v>
+      </c>
+      <c r="J9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="C10" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="J10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="C14" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="C15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="H15" s="25" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="I16" s="16"/>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="C17" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="I17" s="16"/>
+      <c r="J17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="I18" s="16"/>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="I19" s="16"/>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="I20" s="16"/>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="I21" s="16"/>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="C22" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="I22" s="16"/>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="26"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="29"/>
+      <c r="F23" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="G23" s="31"/>
+      <c r="H23" s="32"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="20"/>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="I24" s="16"/>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="I25" s="22"/>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="C26" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F26" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="I26" s="22"/>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="C27" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="I28" s="22"/>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="I29" s="22"/>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="C31" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="C32" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I32" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="C33" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F33" s="13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="C34" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F34" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="C35" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F35" s="13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="C37" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F37" s="13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="C41" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F41" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="J41" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E42" s="2"/>
+      <c r="F42" s="11"/>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="C45" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F45" s="13" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46" s="7" t="s">
+        <v>68</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1066,41 +1609,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1135,7 +1647,7 @@
         <v>33</v>
       </c>
       <c r="G1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="H1" t="s">
         <v>34</v>
@@ -1143,7 +1655,7 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
         <v>35</v>
@@ -1155,18 +1667,18 @@
         <v>36</v>
       </c>
       <c r="E2" t="s">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="F2" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="H2" s="19" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
         <v>35</v>
@@ -1178,18 +1690,18 @@
         <v>36</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H3" s="19" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
         <v>35</v>
@@ -1201,45 +1713,196 @@
         <v>36</v>
       </c>
       <c r="E4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="G4" t="s">
         <v>19</v>
       </c>
       <c r="H4" s="19" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="I4" s="19"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B5" s="20" t="s">
         <v>35</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>102</v>
       </c>
       <c r="D5" t="s">
         <v>36</v>
       </c>
       <c r="E5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F5" t="s">
-        <v>59</v>
-      </c>
-      <c r="G5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H5" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="H5" s="19" t="s">
-        <v>60</v>
-      </c>
       <c r="I5" s="20"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G6" t="s">
+        <v>76</v>
+      </c>
+      <c r="H6" s="19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G7" t="s">
+        <v>78</v>
+      </c>
+      <c r="H7" s="19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>103</v>
+      </c>
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" t="s">
+        <v>75</v>
+      </c>
+      <c r="F8" t="s">
+        <v>55</v>
+      </c>
+      <c r="G8" t="s">
+        <v>52</v>
+      </c>
+      <c r="H8" s="19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" t="s">
+        <v>97</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1268,7 +1931,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="21" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B1" s="21" t="s">
         <v>0</v>
@@ -1276,7 +1939,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="21" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B2" s="21" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Lots of edits from first week of red cross internship. The html js files probably are not working so just make sure it be thorough
</commit_message>
<xml_diff>
--- a/app/config/tables/deployment/forms/deployment/deployment.xlsx
+++ b/app/config/tables/deployment/forms/deployment/deployment.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="3680" windowWidth="50300" windowHeight="19840" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="20" yWindow="0" windowWidth="28780" windowHeight="16060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="model" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="119">
   <si>
     <t>type</t>
   </si>
@@ -351,6 +351,36 @@
   </si>
   <si>
     <t>data('distribution_id') != ''</t>
+  </si>
+  <si>
+    <t>authorization_name_query</t>
+  </si>
+  <si>
+    <t>authorization_id</t>
+  </si>
+  <si>
+    <t>authorization_id_query</t>
+  </si>
+  <si>
+    <t>authorization_name</t>
+  </si>
+  <si>
+    <t>item_pack_id</t>
+  </si>
+  <si>
+    <t>item_pack_id_query</t>
+  </si>
+  <si>
+    <t>item_pack_name_query</t>
+  </si>
+  <si>
+    <t>item_pack_name</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>is_override</t>
   </si>
 </sst>
 </file>
@@ -526,8 +556,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -602,7 +650,7 @@
     <xf numFmtId="0" fontId="6" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="37">
+  <cellStyles count="55">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -621,6 +669,15 @@
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -639,6 +696,15 @@
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -968,10 +1034,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="26" defaultRowHeight="23" x14ac:dyDescent="0"/>
@@ -1035,6 +1101,54 @@
       </c>
       <c r="B7" s="5" t="s">
         <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -1127,10 +1241,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J46"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="23" x14ac:dyDescent="0"/>
@@ -1292,42 +1406,53 @@
         <v>1</v>
       </c>
     </row>
+    <row r="11" spans="1:10">
+      <c r="C11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="7" t="s">
-        <v>50</v>
+      <c r="C12" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>108</v>
+      <c r="C13" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="C14" s="4" t="s">
-        <v>49</v>
+        <v>40</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>115</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>81</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15" spans="1:10">
-      <c r="C15" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="F15" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="H15" s="25" t="s">
-        <v>91</v>
+      <c r="A15" s="7" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1335,264 +1460,297 @@
         <v>57</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="I16" s="16"/>
+        <v>108</v>
+      </c>
     </row>
     <row r="17" spans="1:10">
       <c r="C17" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>84</v>
+        <v>49</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="I17" s="16"/>
-      <c r="J17" t="b">
-        <v>1</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="I18" s="16"/>
+      <c r="C18" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="H18" s="25" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="7" t="s">
-        <v>88</v>
+        <v>57</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>83</v>
       </c>
       <c r="I19" s="16"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="7" t="s">
-        <v>68</v>
+      <c r="C20" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>86</v>
       </c>
       <c r="I20" s="16"/>
+      <c r="J20" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="7" t="s">
-        <v>67</v>
+        <v>57</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>87</v>
       </c>
       <c r="I21" s="16"/>
     </row>
     <row r="22" spans="1:10">
-      <c r="C22" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F22" s="13" t="s">
-        <v>89</v>
+      <c r="A22" s="7" t="s">
+        <v>88</v>
       </c>
       <c r="I22" s="16"/>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="26"/>
-      <c r="B23" s="27"/>
-      <c r="C23" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="D23" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="E23" s="29"/>
-      <c r="F23" s="30" t="s">
-        <v>100</v>
-      </c>
-      <c r="G23" s="31"/>
-      <c r="H23" s="32"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20"/>
+      <c r="A23" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="I23" s="16"/>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="I24" s="16"/>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="C25" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="I25" s="16"/>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="26"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="E26" s="29"/>
+      <c r="F26" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="G26" s="31"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="20"/>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="I24" s="16"/>
-    </row>
-    <row r="25" spans="1:10">
-      <c r="A25" s="7" t="s">
+      <c r="I27" s="16"/>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I25" s="22"/>
-    </row>
-    <row r="26" spans="1:10">
-      <c r="C26" s="4" t="s">
+      <c r="I28" s="22"/>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="C29" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="F26" s="13" t="s">
+      <c r="F29" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="I26" s="22"/>
-    </row>
-    <row r="27" spans="1:10">
-      <c r="C27" s="4" t="s">
+      <c r="I29" s="22"/>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="C30" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D30" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="E30" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
-      <c r="I28" s="22"/>
-    </row>
-    <row r="29" spans="1:10">
-      <c r="A29" s="7" t="s">
+    <row r="31" spans="1:10">
+      <c r="I31" s="22"/>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="I29" s="22"/>
-    </row>
-    <row r="30" spans="1:10">
-      <c r="A30" s="7" t="s">
+      <c r="I32" s="22"/>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="B33" s="7" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10">
-      <c r="C31" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="F31" s="13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10">
-      <c r="C32" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I32" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10">
-      <c r="C33" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F33" s="13" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:10">
       <c r="C34" s="4" t="s">
-        <v>2</v>
+        <v>49</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="F34" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:10">
       <c r="C35" s="4" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F35" s="13" t="s">
-        <v>66</v>
+        <v>20</v>
+      </c>
+      <c r="I35" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:10">
-      <c r="A36" s="7" t="s">
-        <v>67</v>
+      <c r="C36" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F36" s="13" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="37" spans="1:10">
       <c r="C37" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>84</v>
+        <v>2</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>85</v>
+        <v>21</v>
       </c>
       <c r="F37" s="13" t="s">
-        <v>92</v>
+        <v>64</v>
       </c>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>87</v>
+      <c r="C38" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F38" s="13" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="7" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:10">
-      <c r="A40" s="7" t="s">
-        <v>67</v>
+      <c r="C40" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F40" s="13" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="41" spans="1:10">
-      <c r="C41" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E41" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="F41" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="J41" t="b">
-        <v>1</v>
+      <c r="A41" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="42" spans="1:10">
       <c r="A42" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="E42" s="2"/>
-      <c r="F42" s="11"/>
+        <v>88</v>
+      </c>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="C44" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F44" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="J44" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45" s="7" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="44" spans="1:10">
-      <c r="A44" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10">
-      <c r="C45" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F45" s="13" t="s">
-        <v>107</v>
-      </c>
+      <c r="E45" s="2"/>
+      <c r="F45" s="11"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="C48" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F48" s="13" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" s="7" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1609,10 +1767,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1802,7 +1960,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" ht="18" customHeight="1">
       <c r="A8" t="s">
         <v>103</v>
       </c>
@@ -1825,6 +1983,110 @@
         <v>52</v>
       </c>
       <c r="H8" s="19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" t="s">
+        <v>110</v>
+      </c>
+      <c r="H9" s="19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>109</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" t="s">
+        <v>75</v>
+      </c>
+      <c r="F10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" t="s">
+        <v>112</v>
+      </c>
+      <c r="H10" s="19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" t="s">
+        <v>75</v>
+      </c>
+      <c r="F11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" t="s">
+        <v>113</v>
+      </c>
+      <c r="H11" s="19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>115</v>
+      </c>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" t="s">
+        <v>75</v>
+      </c>
+      <c r="F12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12" t="s">
+        <v>116</v>
+      </c>
+      <c r="H12" s="19" t="s">
         <v>56</v>
       </c>
     </row>

</xml_diff>